<commit_message>
Vita ihany ilay stage xD, soutenance apres demain lol
</commit_message>
<xml_diff>
--- a/example/CCID import example.xlsx
+++ b/example/CCID import example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t xml:space="preserve">Nom</t>
   </si>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">Jaona</t>
   </si>
   <si>
-    <t xml:space="preserve">111001030101</t>
+    <t xml:space="preserve">1107</t>
   </si>
   <si>
     <t xml:space="preserve">0325506338</t>
@@ -55,40 +55,10 @@
     <t xml:space="preserve">Tombovelo</t>
   </si>
   <si>
-    <t xml:space="preserve">111001030102</t>
+    <t xml:space="preserve">1105</t>
   </si>
   <si>
     <t xml:space="preserve">0349857376</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rasoa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manitra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">111001030103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0349101010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Randriamalala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0349404040</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rabetokotany</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Voahangy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0349505050</t>
   </si>
 </sst>
 </file>
@@ -198,24 +168,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -470,119 +440,89 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.91"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>111001030104</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="5" t="n">
-        <v>111001030105</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>